<commit_message>
Updating MadixKo & Test_10_SLS
</commit_message>
<xml_diff>
--- a/UnitTests/TuningCorrector/test_10 Manual SLS/8/180613MadixKo_Test_10_TC_1butanal.xlsx
+++ b/UnitTests/TuningCorrector/test_10 Manual SLS/8/180613MadixKo_Test_10_TC_1butanal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4bda48a8e8bf62b/2021LaneLeeCCIFall2021/Data Analysis/220113_Manual_TuningCorrection_Unit_Test_10/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lanel\OneDrive\2021LaneLeeCCIFall2021\Data Analysis\220222_Manual_TuningCorrection_Unit_Test_10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{8FAFFF76-7F1E-4F57-AA30-C47387B52DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8B096A1-4E89-4B9A-91F9-C25CB5CBB3BC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87273C0D-7821-4365-A3F6-A7A5DE56591B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="40665" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23790" yWindow="930" windowWidth="28800" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="31">
   <si>
     <t>Species</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Note: 1butanal data was taken from the external created refernce pattern. The rest of the molecule data was aquired from the initial measured (NonNist) refence data file</t>
+  </si>
+  <si>
+    <t>Compund</t>
+  </si>
+  <si>
+    <t># of electrons (x)</t>
   </si>
 </sst>
 </file>
@@ -5982,8 +5988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P66" sqref="P66"/>
+    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N67" sqref="N67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6007,22 +6013,19 @@
     <col min="18" max="18" width="17.28515625" customWidth="1"/>
     <col min="19" max="19" width="13" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.5703125" customWidth="1"/>
+    <col min="22" max="22" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
-      <c r="V1" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" s="14">
-        <f>(6*4)+8+8</f>
-        <v>40</v>
-      </c>
-      <c r="X1" s="5">
-        <f t="shared" ref="X1:X7" si="0">(0.6*(W1/14))+0.4</f>
-        <v>2.1142857142857143</v>
+      <c r="V1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
@@ -6032,27 +6035,27 @@
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
       <c r="V2" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="W2" s="14">
-        <f>(6*5)+10+8</f>
-        <v>48</v>
+        <f>(6*4)+8+8</f>
+        <v>40</v>
       </c>
       <c r="X2" s="5">
-        <f t="shared" si="0"/>
-        <v>2.4571428571428569</v>
+        <f>(0.6*(W2/14))+0.4</f>
+        <v>2.1142857142857143</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="V3" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="W3" s="14">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="X3" s="5">
-        <f t="shared" si="0"/>
-        <v>1.5142857142857142</v>
+        <f t="shared" ref="X3:X8" si="0">(0.6*(W3/14))+0.4</f>
+        <v>2.1142857142857143</v>
       </c>
       <c r="Y3" t="s">
         <v>2</v>
@@ -6060,14 +6063,14 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="V4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W4" s="14">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="X4" s="5">
         <f t="shared" si="0"/>
-        <v>0.82857142857142851</v>
+        <v>1.5142857142857142</v>
       </c>
       <c r="Y4" t="s">
         <v>4</v>
@@ -6075,14 +6078,14 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="V5" s="9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="W5" s="14">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="X5" s="5">
         <f t="shared" si="0"/>
-        <v>1.342857142857143</v>
+        <v>0.82857142857142851</v>
       </c>
       <c r="Y5" t="s">
         <v>3</v>
@@ -6090,57 +6093,67 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="V6" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="W6" s="14">
-        <f>6+6+4+8</f>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="X6" s="5">
         <f t="shared" si="0"/>
-        <v>1.4285714285714284</v>
+        <v>1.342857142857143</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="V7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="W7" s="14">
+        <f>6+6+4+8</f>
         <v>24</v>
-      </c>
-      <c r="W7" s="14">
-        <f>6+6+4</f>
-        <v>16</v>
       </c>
       <c r="X7" s="5">
         <f t="shared" si="0"/>
-        <v>1.0857142857142856</v>
+        <v>1.4285714285714284</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="V8" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="W8" s="14">
-        <v>14</v>
+        <f>6+6+4</f>
+        <v>16</v>
       </c>
       <c r="X8" s="5">
-        <f>(0.6*(W8/14))+0.4</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>1.0857142857142856</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="V9" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="W9" s="18">
-        <v>2</v>
+      <c r="V9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="W9" s="14">
+        <v>14</v>
       </c>
       <c r="X9" s="5">
         <f>(0.6*(W9/14))+0.4</f>
-        <v>0.48571428571428571</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>5</v>
+      </c>
+      <c r="V10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="W10" s="18">
+        <v>2</v>
+      </c>
+      <c r="X10" s="5">
+        <f>(0.6*(W10/14))+0.4</f>
+        <v>0.48571428571428571</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -8952,11 +8965,11 @@
         <v>19</v>
       </c>
       <c r="C54" s="16" t="e">
-        <f>+ $S65/($X1*C12)</f>
+        <f t="shared" ref="C54:AK54" si="16">+ $S65/($X2*C12)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D54" s="16" t="e">
-        <f t="shared" ref="D54:AK54" si="16">+ $S65/($X1*D12)</f>
+        <f t="shared" si="16"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E54" s="16">
@@ -9097,7 +9110,7 @@
         <v>20</v>
       </c>
       <c r="C55" s="16" t="e">
-        <f t="shared" ref="C55:AK55" si="17">+ $S66/($X2*C13)</f>
+        <f t="shared" ref="C55:AK55" si="17">+ $S66/($X3*C13)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D55" s="16" t="e">
@@ -9106,7 +9119,7 @@
       </c>
       <c r="E55" s="16">
         <f t="shared" si="17"/>
-        <v>59.710290873806038</v>
+        <v>69.393040745234032</v>
       </c>
       <c r="F55" s="16" t="e">
         <f t="shared" si="17"/>
@@ -9126,19 +9139,19 @@
       </c>
       <c r="J55" s="16">
         <f t="shared" si="17"/>
-        <v>47.76823269904483</v>
+        <v>55.514432596187227</v>
       </c>
       <c r="K55" s="16">
         <f t="shared" si="17"/>
-        <v>4.9758575728171701</v>
+        <v>5.7827533954361687</v>
       </c>
       <c r="L55" s="16">
         <f t="shared" si="17"/>
-        <v>19.90343029126868</v>
+        <v>23.131013581744675</v>
       </c>
       <c r="M55" s="16">
         <f t="shared" si="17"/>
-        <v>5.307581411004981</v>
+        <v>6.1682702884652478</v>
       </c>
       <c r="N55" s="16" t="e">
         <f t="shared" si="17"/>
@@ -9158,11 +9171,11 @@
       </c>
       <c r="R55" s="16">
         <f t="shared" si="17"/>
-        <v>59.710290873806038</v>
+        <v>69.393040745234032</v>
       </c>
       <c r="S55" s="16">
         <f t="shared" si="17"/>
-        <v>11.373388737867817</v>
+        <v>13.217722046711245</v>
       </c>
       <c r="T55" s="16" t="e">
         <f t="shared" si="17"/>
@@ -9170,19 +9183,19 @@
       </c>
       <c r="U55" s="16">
         <f t="shared" si="17"/>
-        <v>4.1179510947452433</v>
+        <v>4.7857269479471745</v>
       </c>
       <c r="V55" s="16">
         <f t="shared" si="17"/>
-        <v>19.90343029126868</v>
+        <v>23.131013581744675</v>
       </c>
       <c r="W55" s="16">
         <f t="shared" si="17"/>
-        <v>3.1018332921457681</v>
+        <v>3.6048332854667029</v>
       </c>
       <c r="X55" s="16">
         <f t="shared" si="17"/>
-        <v>2.3884116349522415</v>
+        <v>2.775721629809361</v>
       </c>
       <c r="Y55" s="16" t="e">
         <f t="shared" si="17"/>
@@ -9214,7 +9227,7 @@
       </c>
       <c r="AF55" s="16">
         <f t="shared" si="17"/>
-        <v>7.2376110150067925</v>
+        <v>8.4112776660889743</v>
       </c>
       <c r="AG55" s="16" t="e">
         <f t="shared" si="17"/>
@@ -9242,7 +9255,7 @@
         <v>21</v>
       </c>
       <c r="C56" s="16" t="e">
-        <f t="shared" ref="C56:AK56" si="18">+ $S67/($X3*C14)</f>
+        <f t="shared" ref="C56:AK56" si="18">+ $S67/($X4*C14)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D56" s="16" t="e">
@@ -9387,7 +9400,7 @@
         <v>22</v>
       </c>
       <c r="C57" s="16" t="e">
-        <f t="shared" ref="C57:AK57" si="19">+ $S68/($X4*C15)</f>
+        <f t="shared" ref="C57:AK57" si="19">+ $S68/($X5*C15)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D57" s="16" t="e">
@@ -9532,7 +9545,7 @@
         <v>25</v>
       </c>
       <c r="C58" s="16" t="e">
-        <f t="shared" ref="C58:AK58" si="20">+ $S69/($X5*C16)</f>
+        <f t="shared" ref="C58:AK58" si="20">+ $S69/($X6*C16)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D58" s="16">
@@ -9677,7 +9690,7 @@
         <v>23</v>
       </c>
       <c r="C59" s="16" t="e">
-        <f t="shared" ref="C59:AK59" si="21">+ $S70/($X6*C17)</f>
+        <f t="shared" ref="C59:AK59" si="21">+ $S70/($X7*C17)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D59" s="16" t="e">
@@ -9822,7 +9835,7 @@
         <v>24</v>
       </c>
       <c r="C60" s="16" t="e">
-        <f t="shared" ref="C60:AK60" si="22">+ $S71/($X7*C18)</f>
+        <f t="shared" ref="C60:AK60" si="22">+ $S71/($X8*C18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D60" s="16" t="e">
@@ -9967,7 +9980,7 @@
         <v>26</v>
       </c>
       <c r="C61" s="16" t="e">
-        <f t="shared" ref="C61:AK61" si="23">+ $S72/($X8*C19)</f>
+        <f t="shared" ref="C61:AK61" si="23">+ $S72/($X9*C19)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D61" s="16">
@@ -10112,7 +10125,7 @@
         <v>27</v>
       </c>
       <c r="C62" s="16">
-        <f t="shared" ref="C62:AK62" si="24">+ $S73/($X9*C20)</f>
+        <f t="shared" ref="C62:AK62" si="24">+ $S73/($X10*C20)</f>
         <v>0.55024373334910903</v>
       </c>
       <c r="D62" s="16" t="e">
@@ -10273,7 +10286,7 @@
         <v>19</v>
       </c>
       <c r="S65">
-        <f t="shared" ref="S65:S73" si="25">+SUM(C42:AK42)</f>
+        <f>+SUM(C42:AK42)</f>
         <v>897.88808648341012</v>
       </c>
     </row>
@@ -10301,7 +10314,7 @@
         <v>20</v>
       </c>
       <c r="S66">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="S66:S73" si="25">+SUM(C43:AK43)</f>
         <v>586.86685887397925</v>
       </c>
     </row>
@@ -10343,7 +10356,7 @@
         <v>39</v>
       </c>
       <c r="D68" s="23">
-        <v>11.373388737867817</v>
+        <v>13.217722046711245</v>
       </c>
       <c r="H68" s="9" t="s">
         <v>20</v>
@@ -10355,7 +10368,7 @@
       </c>
       <c r="K68" s="22">
         <f t="shared" ref="K68:K75" si="27">ROUND(D68,1)</f>
-        <v>11.4</v>
+        <v>13.2</v>
       </c>
       <c r="R68" s="9" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Updating Unit Test "test_10.py" Manual SLS
</commit_message>
<xml_diff>
--- a/UnitTests/TuningCorrector/test_10 Manual SLS/8/180613MadixKo_Test_10_TC_1butanal.xlsx
+++ b/UnitTests/TuningCorrector/test_10 Manual SLS/8/180613MadixKo_Test_10_TC_1butanal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4bda48a8e8bf62b/2021LaneLeeCCIFall2021/Data Analysis/220113_Manual_TuningCorrection_Unit_Test_10/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lanel\OneDrive\2021LaneLeeCCIFall2021\Data Analysis\220222_Manual_TuningCorrection_Unit_Test_10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{8FAFFF76-7F1E-4F57-AA30-C47387B52DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8B096A1-4E89-4B9A-91F9-C25CB5CBB3BC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87273C0D-7821-4365-A3F6-A7A5DE56591B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="40665" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23790" yWindow="930" windowWidth="28800" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="31">
   <si>
     <t>Species</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Note: 1butanal data was taken from the external created refernce pattern. The rest of the molecule data was aquired from the initial measured (NonNist) refence data file</t>
+  </si>
+  <si>
+    <t>Compund</t>
+  </si>
+  <si>
+    <t># of electrons (x)</t>
   </si>
 </sst>
 </file>
@@ -5982,8 +5988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P66" sqref="P66"/>
+    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N67" sqref="N67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6007,22 +6013,19 @@
     <col min="18" max="18" width="17.28515625" customWidth="1"/>
     <col min="19" max="19" width="13" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.5703125" customWidth="1"/>
+    <col min="22" max="22" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
-      <c r="V1" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" s="14">
-        <f>(6*4)+8+8</f>
-        <v>40</v>
-      </c>
-      <c r="X1" s="5">
-        <f t="shared" ref="X1:X7" si="0">(0.6*(W1/14))+0.4</f>
-        <v>2.1142857142857143</v>
+      <c r="V1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
@@ -6032,27 +6035,27 @@
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
       <c r="V2" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="W2" s="14">
-        <f>(6*5)+10+8</f>
-        <v>48</v>
+        <f>(6*4)+8+8</f>
+        <v>40</v>
       </c>
       <c r="X2" s="5">
-        <f t="shared" si="0"/>
-        <v>2.4571428571428569</v>
+        <f>(0.6*(W2/14))+0.4</f>
+        <v>2.1142857142857143</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="V3" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="W3" s="14">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="X3" s="5">
-        <f t="shared" si="0"/>
-        <v>1.5142857142857142</v>
+        <f t="shared" ref="X3:X8" si="0">(0.6*(W3/14))+0.4</f>
+        <v>2.1142857142857143</v>
       </c>
       <c r="Y3" t="s">
         <v>2</v>
@@ -6060,14 +6063,14 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="V4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W4" s="14">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="X4" s="5">
         <f t="shared" si="0"/>
-        <v>0.82857142857142851</v>
+        <v>1.5142857142857142</v>
       </c>
       <c r="Y4" t="s">
         <v>4</v>
@@ -6075,14 +6078,14 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="V5" s="9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="W5" s="14">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="X5" s="5">
         <f t="shared" si="0"/>
-        <v>1.342857142857143</v>
+        <v>0.82857142857142851</v>
       </c>
       <c r="Y5" t="s">
         <v>3</v>
@@ -6090,57 +6093,67 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="V6" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="W6" s="14">
-        <f>6+6+4+8</f>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="X6" s="5">
         <f t="shared" si="0"/>
-        <v>1.4285714285714284</v>
+        <v>1.342857142857143</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="V7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="W7" s="14">
+        <f>6+6+4+8</f>
         <v>24</v>
-      </c>
-      <c r="W7" s="14">
-        <f>6+6+4</f>
-        <v>16</v>
       </c>
       <c r="X7" s="5">
         <f t="shared" si="0"/>
-        <v>1.0857142857142856</v>
+        <v>1.4285714285714284</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="V8" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="W8" s="14">
-        <v>14</v>
+        <f>6+6+4</f>
+        <v>16</v>
       </c>
       <c r="X8" s="5">
-        <f>(0.6*(W8/14))+0.4</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>1.0857142857142856</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="V9" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="W9" s="18">
-        <v>2</v>
+      <c r="V9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="W9" s="14">
+        <v>14</v>
       </c>
       <c r="X9" s="5">
         <f>(0.6*(W9/14))+0.4</f>
-        <v>0.48571428571428571</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>5</v>
+      </c>
+      <c r="V10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="W10" s="18">
+        <v>2</v>
+      </c>
+      <c r="X10" s="5">
+        <f>(0.6*(W10/14))+0.4</f>
+        <v>0.48571428571428571</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -8952,11 +8965,11 @@
         <v>19</v>
       </c>
       <c r="C54" s="16" t="e">
-        <f>+ $S65/($X1*C12)</f>
+        <f t="shared" ref="C54:AK54" si="16">+ $S65/($X2*C12)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D54" s="16" t="e">
-        <f t="shared" ref="D54:AK54" si="16">+ $S65/($X1*D12)</f>
+        <f t="shared" si="16"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E54" s="16">
@@ -9097,7 +9110,7 @@
         <v>20</v>
       </c>
       <c r="C55" s="16" t="e">
-        <f t="shared" ref="C55:AK55" si="17">+ $S66/($X2*C13)</f>
+        <f t="shared" ref="C55:AK55" si="17">+ $S66/($X3*C13)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D55" s="16" t="e">
@@ -9106,7 +9119,7 @@
       </c>
       <c r="E55" s="16">
         <f t="shared" si="17"/>
-        <v>59.710290873806038</v>
+        <v>69.393040745234032</v>
       </c>
       <c r="F55" s="16" t="e">
         <f t="shared" si="17"/>
@@ -9126,19 +9139,19 @@
       </c>
       <c r="J55" s="16">
         <f t="shared" si="17"/>
-        <v>47.76823269904483</v>
+        <v>55.514432596187227</v>
       </c>
       <c r="K55" s="16">
         <f t="shared" si="17"/>
-        <v>4.9758575728171701</v>
+        <v>5.7827533954361687</v>
       </c>
       <c r="L55" s="16">
         <f t="shared" si="17"/>
-        <v>19.90343029126868</v>
+        <v>23.131013581744675</v>
       </c>
       <c r="M55" s="16">
         <f t="shared" si="17"/>
-        <v>5.307581411004981</v>
+        <v>6.1682702884652478</v>
       </c>
       <c r="N55" s="16" t="e">
         <f t="shared" si="17"/>
@@ -9158,11 +9171,11 @@
       </c>
       <c r="R55" s="16">
         <f t="shared" si="17"/>
-        <v>59.710290873806038</v>
+        <v>69.393040745234032</v>
       </c>
       <c r="S55" s="16">
         <f t="shared" si="17"/>
-        <v>11.373388737867817</v>
+        <v>13.217722046711245</v>
       </c>
       <c r="T55" s="16" t="e">
         <f t="shared" si="17"/>
@@ -9170,19 +9183,19 @@
       </c>
       <c r="U55" s="16">
         <f t="shared" si="17"/>
-        <v>4.1179510947452433</v>
+        <v>4.7857269479471745</v>
       </c>
       <c r="V55" s="16">
         <f t="shared" si="17"/>
-        <v>19.90343029126868</v>
+        <v>23.131013581744675</v>
       </c>
       <c r="W55" s="16">
         <f t="shared" si="17"/>
-        <v>3.1018332921457681</v>
+        <v>3.6048332854667029</v>
       </c>
       <c r="X55" s="16">
         <f t="shared" si="17"/>
-        <v>2.3884116349522415</v>
+        <v>2.775721629809361</v>
       </c>
       <c r="Y55" s="16" t="e">
         <f t="shared" si="17"/>
@@ -9214,7 +9227,7 @@
       </c>
       <c r="AF55" s="16">
         <f t="shared" si="17"/>
-        <v>7.2376110150067925</v>
+        <v>8.4112776660889743</v>
       </c>
       <c r="AG55" s="16" t="e">
         <f t="shared" si="17"/>
@@ -9242,7 +9255,7 @@
         <v>21</v>
       </c>
       <c r="C56" s="16" t="e">
-        <f t="shared" ref="C56:AK56" si="18">+ $S67/($X3*C14)</f>
+        <f t="shared" ref="C56:AK56" si="18">+ $S67/($X4*C14)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D56" s="16" t="e">
@@ -9387,7 +9400,7 @@
         <v>22</v>
       </c>
       <c r="C57" s="16" t="e">
-        <f t="shared" ref="C57:AK57" si="19">+ $S68/($X4*C15)</f>
+        <f t="shared" ref="C57:AK57" si="19">+ $S68/($X5*C15)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D57" s="16" t="e">
@@ -9532,7 +9545,7 @@
         <v>25</v>
       </c>
       <c r="C58" s="16" t="e">
-        <f t="shared" ref="C58:AK58" si="20">+ $S69/($X5*C16)</f>
+        <f t="shared" ref="C58:AK58" si="20">+ $S69/($X6*C16)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D58" s="16">
@@ -9677,7 +9690,7 @@
         <v>23</v>
       </c>
       <c r="C59" s="16" t="e">
-        <f t="shared" ref="C59:AK59" si="21">+ $S70/($X6*C17)</f>
+        <f t="shared" ref="C59:AK59" si="21">+ $S70/($X7*C17)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D59" s="16" t="e">
@@ -9822,7 +9835,7 @@
         <v>24</v>
       </c>
       <c r="C60" s="16" t="e">
-        <f t="shared" ref="C60:AK60" si="22">+ $S71/($X7*C18)</f>
+        <f t="shared" ref="C60:AK60" si="22">+ $S71/($X8*C18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D60" s="16" t="e">
@@ -9967,7 +9980,7 @@
         <v>26</v>
       </c>
       <c r="C61" s="16" t="e">
-        <f t="shared" ref="C61:AK61" si="23">+ $S72/($X8*C19)</f>
+        <f t="shared" ref="C61:AK61" si="23">+ $S72/($X9*C19)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D61" s="16">
@@ -10112,7 +10125,7 @@
         <v>27</v>
       </c>
       <c r="C62" s="16">
-        <f t="shared" ref="C62:AK62" si="24">+ $S73/($X9*C20)</f>
+        <f t="shared" ref="C62:AK62" si="24">+ $S73/($X10*C20)</f>
         <v>0.55024373334910903</v>
       </c>
       <c r="D62" s="16" t="e">
@@ -10273,7 +10286,7 @@
         <v>19</v>
       </c>
       <c r="S65">
-        <f t="shared" ref="S65:S73" si="25">+SUM(C42:AK42)</f>
+        <f>+SUM(C42:AK42)</f>
         <v>897.88808648341012</v>
       </c>
     </row>
@@ -10301,7 +10314,7 @@
         <v>20</v>
       </c>
       <c r="S66">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="S66:S73" si="25">+SUM(C43:AK43)</f>
         <v>586.86685887397925</v>
       </c>
     </row>
@@ -10343,7 +10356,7 @@
         <v>39</v>
       </c>
       <c r="D68" s="23">
-        <v>11.373388737867817</v>
+        <v>13.217722046711245</v>
       </c>
       <c r="H68" s="9" t="s">
         <v>20</v>
@@ -10355,7 +10368,7 @@
       </c>
       <c r="K68" s="22">
         <f t="shared" ref="K68:K75" si="27">ROUND(D68,1)</f>
-        <v>11.4</v>
+        <v>13.2</v>
       </c>
       <c r="R68" s="9" t="s">
         <v>22</v>

</xml_diff>